<commit_message>
Use ISO date formats
</commit_message>
<xml_diff>
--- a/visit planning/data-template.xlsx
+++ b/visit planning/data-template.xlsx
@@ -530,14 +530,14 @@
     <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="1" errorTitle="Unknown reason for exclusion" error="Please enter this reason in the Exclusions tab first" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>Exclusions!$A:$A</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showDropDown="1" errorTitle="Unknown task" error="Please enter this task in the Tasks tab first" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
-      <formula1>Tasks!$A:$A</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" errorTitle="Unknown subject ID" error="Please enter this subject in the Participants tab first" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+      <formula1>Participants!$A:$A</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showDropDown="1" errorTitle="Invalid release level" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>Predefined!$A$2:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" errorTitle="Unknown subject ID" error="Please enter this subject in the Participants tab first" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
-      <formula1>Participants!$A:$A</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showDropDown="1" errorTitle="Unknown task" error="Please enter this task in the Tasks tab first" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+      <formula1>Tasks!$A:$A</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showDropDown="1" errorTitle="Unknown condition" error="Please enter this condition in the Conditions tab first." showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>Conditions!$A:$A</formula1>
@@ -557,7 +557,7 @@
   <dimension ref="A1:IV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -859,14 +859,14 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showDropDown="1" errorTitle="Unknown ethnicity" error="Are you sure this in the correct ethnicity?" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
-      <formula1>Predefined!$D$2:$D$3</formula1>
-    </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showDropDown="1" errorTitle="Unknown Race" error="Are you sure this is the correct race?" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>Predefined!$C$2:$C$7</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" showDropDown="1" errorTitle="Unknown gender" error="Are you sure this is the correct gender?" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
       <formula1>Predefined!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showDropDown="1" errorTitle="Unknown ethnicity" error="Are you sure this in the correct ethnicity?" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+      <formula1>Predefined!$D$2:$D$3</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -883,7 +883,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -933,7 +933,7 @@
   <dimension ref="A1:IV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:IV1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:IV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A65536"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1503,7 +1503,7 @@
   <dimension ref="A1:IV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:IV1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1790,7 +1790,7 @@
   <dimension ref="A1:IV4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:IV1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2090,7 +2090,7 @@
   <dimension ref="A1:XFD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>